<commit_message>
marc updated diary (#258)
</commit_message>
<xml_diff>
--- a/diaries/diary-marc-andrada.xlsx
+++ b/diaries/diary-marc-andrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marc/Desktop/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F4D71E-E3E4-8B42-ABF0-D5A33BDCBE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72E49BE-EE1C-3A42-A2FC-87ABF47D053C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="25600" windowHeight="14200" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25600" windowHeight="14200" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t>&lt;Happy&gt;</t>
+  </si>
+  <si>
+    <t>&lt;02/05/2020&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Working on assignment 2 for our group project&gt;</t>
+  </si>
+  <si>
+    <t>&lt;We were able to delve deeper into our system and find two features we felt were essential. We created a report of these two features with some image examples.&gt;</t>
+  </si>
+  <si>
+    <t>&lt;This assignment helped us to really hone in on our reverse-engineering skills acquired thus far. We used a top down method to determine features we believed would be essential. There was a lot of conversation among my team members as to whether extended components of these features should be included or not, which was good&gt;</t>
+  </si>
+  <si>
+    <t>&lt;A little sleepy, but nothing some coffee cant fix :]&gt;</t>
   </si>
 </sst>
 </file>
@@ -662,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -904,14 +919,28 @@
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
+    <row r="16" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>

</xml_diff>